<commit_message>
On branch jg-docker-01 Your branch is up to date with 'origin/jg-docker-01'.
Changes to be committed:
	new file:   network-analytics-final/notebooks/shap-lime-anaylisis.ipynb
	modified:   network-analytics-final/powerpoint/Network Analysis - MLE Capstone Presentation_v07.pptx
	modified:   network-analytics-final/powerpoint/excel-for-tables.xlsx
	deleted:    network-analytics-final/powerpoint/~$Network Analysis - MLE Capstone Presentation_v07.pptx
</commit_message>
<xml_diff>
--- a/network-analytics-final/powerpoint/excel-for-tables.xlsx
+++ b/network-analytics-final/powerpoint/excel-for-tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaquingianantonio/Dropbox/FIUBA/Phyton/Fourth_Brain/gitrepo/network-analytics-final/network-analytics-final/powerpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797EAE81-1A92-4040-BD50-CE7F9782DC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE43EF07-D979-2F43-BAA4-5D12DBF4E9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{E9ED5C6B-E51D-1F44-BA09-60D604BE9C82}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>TCP - SYN</t>
   </si>
@@ -211,12 +211,30 @@
   <si>
     <t>Multiclass Labels</t>
   </si>
+  <si>
+    <t>Tcp</t>
+  </si>
+  <si>
+    <t>blac,</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>over</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -277,6 +295,12 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -420,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -457,6 +481,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA384A7-296A-4B4A-9FCD-9EF219F3F587}">
-  <dimension ref="B4:Z13335"/>
+  <dimension ref="B2:AJ13335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N8" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1030,7 +1055,49 @@
     <col min="26" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:26">
+    <row r="2" spans="2:36">
+      <c r="AC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>7273</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>1808</v>
+      </c>
+      <c r="AI2" s="2">
+        <f>AD2+AG2</f>
+        <v>9081</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:36">
+      <c r="AC3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>6739</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>1681</v>
+      </c>
+      <c r="AI3" s="2">
+        <f t="shared" ref="AI3:AI7" si="0">AD3+AG3</f>
+        <v>8420</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36">
       <c r="D4" s="1"/>
       <c r="G4" s="3">
         <v>0</v>
@@ -1038,8 +1105,27 @@
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:26">
+      <c r="AC4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>4504</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>1111</v>
+      </c>
+      <c r="AI4" s="2">
+        <f t="shared" si="0"/>
+        <v>5615</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36">
       <c r="D5" s="1"/>
       <c r="G5" s="3">
         <v>1</v>
@@ -1047,8 +1133,27 @@
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:26">
+      <c r="AC5" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>3003</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>770</v>
+      </c>
+      <c r="AI5" s="2">
+        <f t="shared" si="0"/>
+        <v>3773</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36">
       <c r="D6" s="1"/>
       <c r="G6" s="3">
         <v>2</v>
@@ -1061,8 +1166,27 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:26">
+      <c r="AC6" s="2">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>820</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>4</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>202</v>
+      </c>
+      <c r="AI6" s="2">
+        <f t="shared" si="0"/>
+        <v>1022</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36">
       <c r="D7" s="1"/>
       <c r="G7" s="3">
         <v>3</v>
@@ -1079,8 +1203,27 @@
         <v>27</v>
       </c>
       <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:26">
+      <c r="AC7" s="30">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>7589</v>
+      </c>
+      <c r="AF7" s="30">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>1911</v>
+      </c>
+      <c r="AI7" s="2">
+        <f t="shared" si="0"/>
+        <v>9500</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36">
       <c r="D8" s="1"/>
       <c r="G8" s="3">
         <v>4</v>
@@ -1098,7 +1241,7 @@
       </c>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="2:26">
+    <row r="9" spans="2:36">
       <c r="D9" s="1"/>
       <c r="G9" s="3">
         <v>5</v>
@@ -1116,7 +1259,7 @@
       </c>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="2:26">
+    <row r="10" spans="2:36">
       <c r="Q10" s="4"/>
       <c r="R10" s="14" t="s">
         <v>12</v>
@@ -1127,7 +1270,7 @@
       </c>
       <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="2:26">
+    <row r="11" spans="2:36">
       <c r="Q11" s="4"/>
       <c r="R11" s="14" t="s">
         <v>14</v>
@@ -1138,7 +1281,7 @@
       </c>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="2:26">
+    <row r="12" spans="2:36">
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1161,7 +1304,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="2:26">
+    <row r="13" spans="2:36">
       <c r="I13" s="4"/>
       <c r="J13" s="10" t="s">
         <v>26</v>
@@ -1190,7 +1333,7 @@
       <c r="Y13" s="26"/>
       <c r="Z13" s="4"/>
     </row>
-    <row r="14" spans="2:26">
+    <row r="14" spans="2:36">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1229,7 +1372,7 @@
       </c>
       <c r="Z14" s="4"/>
     </row>
-    <row r="15" spans="2:26">
+    <row r="15" spans="2:36">
       <c r="B15" s="4"/>
       <c r="C15" s="6" t="s">
         <v>38</v>
@@ -1272,7 +1415,7 @@
       </c>
       <c r="Z15" s="4"/>
     </row>
-    <row r="16" spans="2:26">
+    <row r="16" spans="2:36">
       <c r="B16" s="4"/>
       <c r="C16" s="8" t="s">
         <v>3</v>
@@ -1614,6 +1757,54 @@
         <v>5615</v>
       </c>
     </row>
+    <row r="35" spans="3:4">
+      <c r="C35" s="2">
+        <v>9081</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="C36" s="2">
+        <v>8420</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="C37" s="2">
+        <v>5615</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4">
+      <c r="C38" s="30">
+        <v>3773</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="C39" s="2">
+        <v>1022</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4">
+      <c r="C40" s="2">
+        <v>9500</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="55" spans="14:15">
       <c r="N55" s="23"/>
       <c r="O55" s="24"/>
@@ -54739,6 +54930,9 @@
       <c r="O13335" s="24"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AF2:AG7">
+    <sortCondition ref="AF2:AF7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>